<commit_message>
GR-PII Update all review changes
</commit_message>
<xml_diff>
--- a/DHL/Template/20230405_NEW SIR_GR_Greecev_v2.2.1.xlsx
+++ b/DHL/Template/20230405_NEW SIR_GR_Greecev_v2.2.1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DHL-Master\County\GR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DHL-Master\Git-Master\TestJavaProject\DHL\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -5598,11 +5598,23 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -5618,18 +5630,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -14200,11 +14200,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="D28" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="3" ySplit="4" topLeftCell="D32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H2" sqref="H2"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="G33" sqref="G33"/>
+      <selection pane="bottomRight" activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="44.140625" defaultRowHeight="12.75"/>
@@ -14256,112 +14256,112 @@
       <c r="T1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="15" customHeight="1">
-      <c r="A2" s="146" t="s">
+      <c r="A2" s="139" t="s">
         <v>1018</v>
       </c>
-      <c r="B2" s="143" t="s">
+      <c r="B2" s="147" t="s">
         <v>1019</v>
       </c>
-      <c r="C2" s="144" t="s">
+      <c r="C2" s="148" t="s">
         <v>1020</v>
       </c>
-      <c r="D2" s="145" t="s">
+      <c r="D2" s="149" t="s">
         <v>1222</v>
       </c>
-      <c r="E2" s="145" t="s">
+      <c r="E2" s="149" t="s">
         <v>1223</v>
       </c>
-      <c r="F2" s="145" t="s">
+      <c r="F2" s="149" t="s">
         <v>1224</v>
       </c>
-      <c r="G2" s="145" t="s">
+      <c r="G2" s="149" t="s">
         <v>1225</v>
       </c>
-      <c r="H2" s="141" t="s">
+      <c r="H2" s="145" t="s">
         <v>1021</v>
       </c>
-      <c r="I2" s="141" t="s">
+      <c r="I2" s="145" t="s">
         <v>1022</v>
       </c>
-      <c r="J2" s="148" t="s">
+      <c r="J2" s="143" t="s">
         <v>1023</v>
       </c>
-      <c r="K2" s="148" t="s">
+      <c r="K2" s="143" t="s">
         <v>1024</v>
       </c>
-      <c r="L2" s="148" t="s">
+      <c r="L2" s="143" t="s">
         <v>1025</v>
       </c>
-      <c r="M2" s="148" t="s">
+      <c r="M2" s="143" t="s">
         <v>1026</v>
       </c>
-      <c r="N2" s="148" t="s">
+      <c r="N2" s="143" t="s">
         <v>1027</v>
       </c>
-      <c r="O2" s="139" t="s">
+      <c r="O2" s="141" t="s">
         <v>1028</v>
       </c>
-      <c r="P2" s="139" t="s">
+      <c r="P2" s="141" t="s">
         <v>1029</v>
       </c>
-      <c r="Q2" s="139" t="s">
+      <c r="Q2" s="141" t="s">
         <v>1030</v>
       </c>
-      <c r="R2" s="148" t="s">
+      <c r="R2" s="143" t="s">
         <v>1031</v>
       </c>
-      <c r="S2" s="139" t="s">
+      <c r="S2" s="141" t="s">
         <v>1032</v>
       </c>
-      <c r="T2" s="139" t="s">
+      <c r="T2" s="141" t="s">
         <v>1033</v>
       </c>
-      <c r="U2" s="139" t="s">
+      <c r="U2" s="141" t="s">
         <v>1034</v>
       </c>
-      <c r="V2" s="139" t="s">
+      <c r="V2" s="141" t="s">
         <v>1035</v>
       </c>
-      <c r="W2" s="139" t="s">
+      <c r="W2" s="141" t="s">
         <v>1036</v>
       </c>
-      <c r="X2" s="139" t="s">
+      <c r="X2" s="141" t="s">
         <v>1037</v>
       </c>
-      <c r="Y2" s="139" t="s">
+      <c r="Y2" s="141" t="s">
         <v>1038</v>
       </c>
-      <c r="Z2" s="139" t="s">
+      <c r="Z2" s="141" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:26">
-      <c r="A3" s="147"/>
-      <c r="B3" s="143"/>
-      <c r="C3" s="144"/>
-      <c r="D3" s="145"/>
-      <c r="E3" s="145"/>
-      <c r="F3" s="145"/>
-      <c r="G3" s="145"/>
-      <c r="H3" s="142"/>
-      <c r="I3" s="142"/>
-      <c r="J3" s="149"/>
-      <c r="K3" s="149"/>
-      <c r="L3" s="149"/>
-      <c r="M3" s="149"/>
-      <c r="N3" s="149"/>
-      <c r="O3" s="140"/>
-      <c r="P3" s="140"/>
-      <c r="Q3" s="140"/>
-      <c r="R3" s="149"/>
-      <c r="S3" s="140"/>
-      <c r="T3" s="140"/>
-      <c r="U3" s="140"/>
-      <c r="V3" s="140"/>
-      <c r="W3" s="140"/>
-      <c r="X3" s="140"/>
-      <c r="Y3" s="140"/>
-      <c r="Z3" s="140"/>
+      <c r="A3" s="140"/>
+      <c r="B3" s="147"/>
+      <c r="C3" s="148"/>
+      <c r="D3" s="149"/>
+      <c r="E3" s="149"/>
+      <c r="F3" s="149"/>
+      <c r="G3" s="149"/>
+      <c r="H3" s="146"/>
+      <c r="I3" s="146"/>
+      <c r="J3" s="144"/>
+      <c r="K3" s="144"/>
+      <c r="L3" s="144"/>
+      <c r="M3" s="144"/>
+      <c r="N3" s="144"/>
+      <c r="O3" s="142"/>
+      <c r="P3" s="142"/>
+      <c r="Q3" s="142"/>
+      <c r="R3" s="144"/>
+      <c r="S3" s="142"/>
+      <c r="T3" s="142"/>
+      <c r="U3" s="142"/>
+      <c r="V3" s="142"/>
+      <c r="W3" s="142"/>
+      <c r="X3" s="142"/>
+      <c r="Y3" s="142"/>
+      <c r="Z3" s="142"/>
     </row>
     <row r="4" spans="1:26" ht="63.75">
       <c r="A4" s="4"/>
@@ -16269,6 +16269,16 @@
   </sheetData>
   <autoFilter ref="A1:Z51"/>
   <mergeCells count="26">
+    <mergeCell ref="V2:V3"/>
+    <mergeCell ref="X2:X3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="U2:U3"/>
     <mergeCell ref="W2:W3"/>
@@ -16285,16 +16295,6 @@
     <mergeCell ref="Q2:Q3"/>
     <mergeCell ref="R2:R3"/>
     <mergeCell ref="S2:S3"/>
-    <mergeCell ref="V2:V3"/>
-    <mergeCell ref="X2:X3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="T7" r:id="rId1" display="https://ec.europa.eu/taxation_customs/dds2/eos/eori_validation.jsp?Lang=en&amp;EoriNumb=GR123456789&amp;Expand=true"/>
@@ -16337,21 +16337,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E4B081E47C8C644A96CCB2DD9F6CA5F4" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d3b26137e7259a2446488c7e73176ed5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a38bb563-b043-4e2c-865d-7b7896bda23c" xmlns:ns3="abd88cbd-128a-4215-be95-828ed75d5cc4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ac9625e74072deb930559480f217758b" ns2:_="" ns3:_="">
     <xsd:import namespace="a38bb563-b043-4e2c-865d-7b7896bda23c"/>
@@ -16534,24 +16519,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B080708-15F3-4B11-B7E8-C333FE45C4FF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C7354AF-45C3-4ABE-9306-B33138299E90}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44364AE4-9C15-43CF-9C81-208ACDC7A0E1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -16568,4 +16551,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C7354AF-45C3-4ABE-9306-B33138299E90}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B080708-15F3-4B11-B7E8-C333FE45C4FF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
GR-PII json Configuration changes updated
</commit_message>
<xml_diff>
--- a/DHL/Template/20230405_NEW SIR_GR_Greecev_v2.2.1.xlsx
+++ b/DHL/Template/20230405_NEW SIR_GR_Greecev_v2.2.1.xlsx
@@ -4737,9 +4737,6 @@
     <t>SIR Name</t>
   </si>
   <si>
-    <t>PORadioBtn</t>
-  </si>
-  <si>
     <t>RetExport</t>
   </si>
   <si>
@@ -4777,6 +4774,9 @@
   </si>
   <si>
     <t>InvUploader</t>
+  </si>
+  <si>
+    <t>GRVatBtn</t>
   </si>
 </sst>
 </file>
@@ -5598,23 +5598,11 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -5630,6 +5618,18 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -14201,10 +14201,10 @@
   <dimension ref="A1:Z51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="D32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="4" topLeftCell="P21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H2" sqref="H2"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="F36" sqref="F36"/>
+      <selection pane="bottomRight" activeCell="U24" sqref="U24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="44.140625" defaultRowHeight="12.75"/>
@@ -14256,112 +14256,112 @@
       <c r="T1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="15" customHeight="1">
-      <c r="A2" s="139" t="s">
+      <c r="A2" s="146" t="s">
         <v>1018</v>
       </c>
-      <c r="B2" s="147" t="s">
+      <c r="B2" s="143" t="s">
         <v>1019</v>
       </c>
-      <c r="C2" s="148" t="s">
+      <c r="C2" s="144" t="s">
         <v>1020</v>
       </c>
-      <c r="D2" s="149" t="s">
+      <c r="D2" s="145" t="s">
         <v>1222</v>
       </c>
-      <c r="E2" s="149" t="s">
+      <c r="E2" s="145" t="s">
         <v>1223</v>
       </c>
-      <c r="F2" s="149" t="s">
+      <c r="F2" s="145" t="s">
         <v>1224</v>
       </c>
-      <c r="G2" s="149" t="s">
+      <c r="G2" s="145" t="s">
         <v>1225</v>
       </c>
-      <c r="H2" s="145" t="s">
+      <c r="H2" s="141" t="s">
         <v>1021</v>
       </c>
-      <c r="I2" s="145" t="s">
+      <c r="I2" s="141" t="s">
         <v>1022</v>
       </c>
-      <c r="J2" s="143" t="s">
+      <c r="J2" s="148" t="s">
         <v>1023</v>
       </c>
-      <c r="K2" s="143" t="s">
+      <c r="K2" s="148" t="s">
         <v>1024</v>
       </c>
-      <c r="L2" s="143" t="s">
+      <c r="L2" s="148" t="s">
         <v>1025</v>
       </c>
-      <c r="M2" s="143" t="s">
+      <c r="M2" s="148" t="s">
         <v>1026</v>
       </c>
-      <c r="N2" s="143" t="s">
+      <c r="N2" s="148" t="s">
         <v>1027</v>
       </c>
-      <c r="O2" s="141" t="s">
+      <c r="O2" s="139" t="s">
         <v>1028</v>
       </c>
-      <c r="P2" s="141" t="s">
+      <c r="P2" s="139" t="s">
         <v>1029</v>
       </c>
-      <c r="Q2" s="141" t="s">
+      <c r="Q2" s="139" t="s">
         <v>1030</v>
       </c>
-      <c r="R2" s="143" t="s">
+      <c r="R2" s="148" t="s">
         <v>1031</v>
       </c>
-      <c r="S2" s="141" t="s">
+      <c r="S2" s="139" t="s">
         <v>1032</v>
       </c>
-      <c r="T2" s="141" t="s">
+      <c r="T2" s="139" t="s">
         <v>1033</v>
       </c>
-      <c r="U2" s="141" t="s">
+      <c r="U2" s="139" t="s">
         <v>1034</v>
       </c>
-      <c r="V2" s="141" t="s">
+      <c r="V2" s="139" t="s">
         <v>1035</v>
       </c>
-      <c r="W2" s="141" t="s">
+      <c r="W2" s="139" t="s">
         <v>1036</v>
       </c>
-      <c r="X2" s="141" t="s">
+      <c r="X2" s="139" t="s">
         <v>1037</v>
       </c>
-      <c r="Y2" s="141" t="s">
+      <c r="Y2" s="139" t="s">
         <v>1038</v>
       </c>
-      <c r="Z2" s="141" t="s">
+      <c r="Z2" s="139" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:26">
-      <c r="A3" s="140"/>
-      <c r="B3" s="147"/>
-      <c r="C3" s="148"/>
-      <c r="D3" s="149"/>
-      <c r="E3" s="149"/>
-      <c r="F3" s="149"/>
-      <c r="G3" s="149"/>
-      <c r="H3" s="146"/>
-      <c r="I3" s="146"/>
-      <c r="J3" s="144"/>
-      <c r="K3" s="144"/>
-      <c r="L3" s="144"/>
-      <c r="M3" s="144"/>
-      <c r="N3" s="144"/>
-      <c r="O3" s="142"/>
-      <c r="P3" s="142"/>
-      <c r="Q3" s="142"/>
-      <c r="R3" s="144"/>
-      <c r="S3" s="142"/>
-      <c r="T3" s="142"/>
-      <c r="U3" s="142"/>
-      <c r="V3" s="142"/>
-      <c r="W3" s="142"/>
-      <c r="X3" s="142"/>
-      <c r="Y3" s="142"/>
-      <c r="Z3" s="142"/>
+      <c r="A3" s="147"/>
+      <c r="B3" s="143"/>
+      <c r="C3" s="144"/>
+      <c r="D3" s="145"/>
+      <c r="E3" s="145"/>
+      <c r="F3" s="145"/>
+      <c r="G3" s="145"/>
+      <c r="H3" s="142"/>
+      <c r="I3" s="142"/>
+      <c r="J3" s="149"/>
+      <c r="K3" s="149"/>
+      <c r="L3" s="149"/>
+      <c r="M3" s="149"/>
+      <c r="N3" s="149"/>
+      <c r="O3" s="140"/>
+      <c r="P3" s="140"/>
+      <c r="Q3" s="140"/>
+      <c r="R3" s="149"/>
+      <c r="S3" s="140"/>
+      <c r="T3" s="140"/>
+      <c r="U3" s="140"/>
+      <c r="V3" s="140"/>
+      <c r="W3" s="140"/>
+      <c r="X3" s="140"/>
+      <c r="Y3" s="140"/>
+      <c r="Z3" s="140"/>
     </row>
     <row r="4" spans="1:26" ht="63.75">
       <c r="A4" s="4"/>
@@ -15045,7 +15045,7 @@
       <c r="B21" s="41"/>
       <c r="C21" s="46"/>
       <c r="D21" s="46" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="E21" s="46"/>
       <c r="F21" s="46"/>
@@ -15085,10 +15085,10 @@
         <v>1087</v>
       </c>
       <c r="D22" s="46" t="s">
+        <v>1228</v>
+      </c>
+      <c r="E22" s="46" t="s">
         <v>1229</v>
-      </c>
-      <c r="E22" s="46" t="s">
-        <v>1230</v>
       </c>
       <c r="F22" s="46"/>
       <c r="G22" s="46"/>
@@ -15123,10 +15123,10 @@
         <v>1125</v>
       </c>
       <c r="D23" s="46" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="E23" s="46" t="s">
-        <v>1226</v>
+        <v>1239</v>
       </c>
       <c r="F23" s="46"/>
       <c r="G23" s="46"/>
@@ -15161,10 +15161,10 @@
         <v>1128</v>
       </c>
       <c r="D24" s="46" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="E24" s="46" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="F24" s="46"/>
       <c r="G24" s="46"/>
@@ -15211,10 +15211,10 @@
         <v>1134</v>
       </c>
       <c r="D25" s="46" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="E25" s="46" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="F25" s="46"/>
       <c r="G25" s="46"/>
@@ -15327,7 +15327,7 @@
       <c r="B28" s="41"/>
       <c r="C28" s="46"/>
       <c r="D28" s="46" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="E28" s="46"/>
       <c r="F28" s="46"/>
@@ -15367,10 +15367,10 @@
         <v>1150</v>
       </c>
       <c r="D29" s="119" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="E29" s="119" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="F29" s="119"/>
       <c r="G29" s="119"/>
@@ -15405,10 +15405,10 @@
         <v>1153</v>
       </c>
       <c r="D30" s="119" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="E30" s="119" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="F30" s="119"/>
       <c r="G30" s="119"/>
@@ -15445,10 +15445,10 @@
         <v>1157</v>
       </c>
       <c r="D31" s="46" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="E31" s="119" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="F31" s="46"/>
       <c r="G31" s="119"/>
@@ -15489,10 +15489,10 @@
         <v>1157</v>
       </c>
       <c r="D32" s="46" t="s">
+        <v>1226</v>
+      </c>
+      <c r="E32" s="119" t="s">
         <v>1227</v>
-      </c>
-      <c r="E32" s="119" t="s">
-        <v>1228</v>
       </c>
       <c r="F32" s="46"/>
       <c r="G32" s="119"/>
@@ -15531,10 +15531,10 @@
         <v>1162</v>
       </c>
       <c r="D33" s="46" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="E33" s="119" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="F33" s="46"/>
       <c r="G33" s="119"/>
@@ -15571,10 +15571,10 @@
         <v>1165</v>
       </c>
       <c r="D34" s="46" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="E34" s="119" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="F34" s="46"/>
       <c r="G34" s="119"/>
@@ -15615,10 +15615,10 @@
         <v>1157</v>
       </c>
       <c r="D35" s="46" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="E35" s="119" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="F35" s="46"/>
       <c r="G35" s="119"/>
@@ -15657,10 +15657,10 @@
         <v>1171</v>
       </c>
       <c r="D36" s="46" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="E36" s="119" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="F36" s="46"/>
       <c r="G36" s="119"/>
@@ -16269,16 +16269,6 @@
   </sheetData>
   <autoFilter ref="A1:Z51"/>
   <mergeCells count="26">
-    <mergeCell ref="V2:V3"/>
-    <mergeCell ref="X2:X3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="U2:U3"/>
     <mergeCell ref="W2:W3"/>
@@ -16295,6 +16285,16 @@
     <mergeCell ref="Q2:Q3"/>
     <mergeCell ref="R2:R3"/>
     <mergeCell ref="S2:S3"/>
+    <mergeCell ref="V2:V3"/>
+    <mergeCell ref="X2:X3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="T7" r:id="rId1" display="https://ec.europa.eu/taxation_customs/dds2/eos/eori_validation.jsp?Lang=en&amp;EoriNumb=GR123456789&amp;Expand=true"/>
@@ -16337,6 +16337,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E4B081E47C8C644A96CCB2DD9F6CA5F4" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d3b26137e7259a2446488c7e73176ed5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a38bb563-b043-4e2c-865d-7b7896bda23c" xmlns:ns3="abd88cbd-128a-4215-be95-828ed75d5cc4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ac9625e74072deb930559480f217758b" ns2:_="" ns3:_="">
     <xsd:import namespace="a38bb563-b043-4e2c-865d-7b7896bda23c"/>
@@ -16519,22 +16534,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B080708-15F3-4B11-B7E8-C333FE45C4FF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C7354AF-45C3-4ABE-9306-B33138299E90}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44364AE4-9C15-43CF-9C81-208ACDC7A0E1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -16551,21 +16568,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C7354AF-45C3-4ABE-9306-B33138299E90}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B080708-15F3-4B11-B7E8-C333FE45C4FF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>